<commit_message>
Ajuste en clases y funciones
</commit_message>
<xml_diff>
--- a/Jugadores.xlsx
+++ b/Jugadores.xlsx
@@ -531,12 +531,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>08/11/2022 22:00</t>
+          <t>11/11/2022 23:21</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Se incluye registro de wins gato, se integra gato a menus principal y cambos visuales en juegos
</commit_message>
<xml_diff>
--- a/Jugadores.xlsx
+++ b/Jugadores.xlsx
@@ -499,7 +499,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>03/12/2022 15:08</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -526,7 +531,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>03/12/2022 15:17</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -553,7 +563,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>03/12/2022 14:54</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -575,12 +590,22 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>03/12/2022 15:16</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>03/12/2022 14:37</t>
         </is>
       </c>
     </row>

</xml_diff>